<commit_message>
add fill value and plot line function at WCDMA
</commit_message>
<xml_diff>
--- a/results_1.4MHZ_LTE.xlsx
+++ b/results_1.4MHZ_LTE.xlsx
@@ -575,6 +575,8 @@
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
+          <max val="-20"/>
+          <min val="-60"/>
         </scaling>
         <axPos val="l"/>
         <majorGridlines/>
@@ -856,6 +858,8 @@
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
+          <max val="-20"/>
+          <min val="-60"/>
         </scaling>
         <axPos val="l"/>
         <majorGridlines/>
@@ -1137,6 +1141,8 @@
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
+          <max val="-20"/>
+          <min val="-60"/>
         </scaling>
         <axPos val="l"/>
         <majorGridlines/>
@@ -1418,6 +1424,8 @@
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
+          <max val="-20"/>
+          <min val="-60"/>
         </scaling>
         <axPos val="l"/>
         <majorGridlines/>
@@ -3907,6 +3915,8 @@
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
+          <max val="-20"/>
+          <min val="-60"/>
         </scaling>
         <axPos val="l"/>
         <majorGridlines/>
@@ -4188,6 +4198,8 @@
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
+          <max val="-20"/>
+          <min val="-60"/>
         </scaling>
         <axPos val="l"/>
         <majorGridlines/>
@@ -5057,13 +5069,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>24.68</v>
+        <v>24.51</v>
       </c>
       <c r="C2" t="n">
-        <v>24.79</v>
+        <v>24.4</v>
       </c>
       <c r="D2" t="n">
-        <v>24.67</v>
+        <v>24.14</v>
       </c>
     </row>
     <row r="3">
@@ -5071,13 +5083,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>24.91</v>
+        <v>24.33</v>
       </c>
       <c r="C3" t="n">
-        <v>24.85</v>
+        <v>24.43</v>
       </c>
       <c r="D3" t="n">
-        <v>24.83</v>
+        <v>24.36</v>
       </c>
     </row>
     <row r="4">
@@ -5085,13 +5097,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>24.61</v>
+        <v>23.99</v>
       </c>
       <c r="C4" t="n">
-        <v>24.5</v>
+        <v>23.97</v>
       </c>
       <c r="D4" t="n">
-        <v>24.55</v>
+        <v>23.84</v>
       </c>
     </row>
     <row r="5">
@@ -5099,13 +5111,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>24.77</v>
+        <v>24.27</v>
       </c>
       <c r="C5" t="n">
-        <v>24.8</v>
+        <v>24.37</v>
       </c>
       <c r="D5" t="n">
-        <v>24.6</v>
+        <v>24.16</v>
       </c>
     </row>
     <row r="6">
@@ -5113,13 +5125,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>24.88</v>
+        <v>24.22</v>
       </c>
       <c r="C6" t="n">
-        <v>24.9</v>
+        <v>24.2</v>
       </c>
       <c r="D6" t="n">
-        <v>24.94</v>
+        <v>24.32</v>
       </c>
     </row>
   </sheetData>
@@ -5194,16 +5206,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-44.55</v>
+        <v>-46.79</v>
       </c>
       <c r="D2" t="n">
-        <v>-46.2</v>
+        <v>-48.84</v>
       </c>
       <c r="E2" t="n">
-        <v>-47.47</v>
+        <v>-48.89</v>
       </c>
       <c r="F2" t="n">
-        <v>-48.46</v>
+        <v>-49.45</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -5222,16 +5234,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-45.12</v>
+        <v>-45.64</v>
       </c>
       <c r="D3" t="n">
-        <v>-46.53</v>
+        <v>-48.13</v>
       </c>
       <c r="E3" t="n">
-        <v>-47.51</v>
+        <v>-48.58</v>
       </c>
       <c r="F3" t="n">
-        <v>-48.99</v>
+        <v>-50.16</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -5250,16 +5262,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-41.8</v>
+        <v>-42.74</v>
       </c>
       <c r="D4" t="n">
-        <v>-45.27</v>
+        <v>-45.65</v>
       </c>
       <c r="E4" t="n">
-        <v>-46.75</v>
+        <v>-47.13</v>
       </c>
       <c r="F4" t="n">
-        <v>-48.69</v>
+        <v>-48.99</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -5278,16 +5290,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-49.1</v>
+        <v>-45.21</v>
       </c>
       <c r="D5" t="n">
-        <v>-50.1</v>
+        <v>-46.87</v>
       </c>
       <c r="E5" t="n">
-        <v>-49.93</v>
+        <v>-48.27</v>
       </c>
       <c r="F5" t="n">
-        <v>-50.02</v>
+        <v>-49</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -5306,16 +5318,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-47.52</v>
+        <v>-47.14</v>
       </c>
       <c r="D6" t="n">
-        <v>-49.23</v>
+        <v>-49.06</v>
       </c>
       <c r="E6" t="n">
-        <v>-50.01</v>
+        <v>-49.45</v>
       </c>
       <c r="F6" t="n">
-        <v>-50.85</v>
+        <v>-50.45</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -5334,16 +5346,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-44.34</v>
+        <v>-45.24</v>
       </c>
       <c r="D7" t="n">
-        <v>-46.08</v>
+        <v>-47.2</v>
       </c>
       <c r="E7" t="n">
-        <v>-47.21</v>
+        <v>-47.97</v>
       </c>
       <c r="F7" t="n">
-        <v>-49.22</v>
+        <v>-49.75</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -5362,16 +5374,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-48.33</v>
+        <v>-46.57</v>
       </c>
       <c r="D8" t="n">
-        <v>-49.47</v>
+        <v>-47.91</v>
       </c>
       <c r="E8" t="n">
-        <v>-49.94</v>
+        <v>-49.49</v>
       </c>
       <c r="F8" t="n">
-        <v>-49.95</v>
+        <v>-49.83</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -5390,16 +5402,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-45.22</v>
+        <v>-45.04</v>
       </c>
       <c r="D9" t="n">
-        <v>-48.22</v>
+        <v>-48.08</v>
       </c>
       <c r="E9" t="n">
-        <v>-48.22</v>
+        <v>-48.27</v>
       </c>
       <c r="F9" t="n">
-        <v>-49.38</v>
+        <v>-49.47</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -5418,16 +5430,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-41.28</v>
+        <v>-41.37</v>
       </c>
       <c r="D10" t="n">
-        <v>-43.78</v>
+        <v>-43.86</v>
       </c>
       <c r="E10" t="n">
-        <v>-45.51</v>
+        <v>-45.95</v>
       </c>
       <c r="F10" t="n">
-        <v>-46.96</v>
+        <v>-47.94</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -5446,16 +5458,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-42.79</v>
+        <v>-44.63</v>
       </c>
       <c r="D11" t="n">
-        <v>-45.39</v>
+        <v>-46.4</v>
       </c>
       <c r="E11" t="n">
-        <v>-46.84</v>
+        <v>-48.3</v>
       </c>
       <c r="F11" t="n">
-        <v>-48.68</v>
+        <v>-49.42</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -5474,16 +5486,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-46.82</v>
+        <v>-48.51</v>
       </c>
       <c r="D12" t="n">
-        <v>-48.41</v>
+        <v>-50.2</v>
       </c>
       <c r="E12" t="n">
-        <v>-48.72</v>
+        <v>-49.97</v>
       </c>
       <c r="F12" t="n">
-        <v>-49.94</v>
+        <v>-50.86</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -5502,16 +5514,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-41.49</v>
+        <v>-42.32</v>
       </c>
       <c r="D13" t="n">
-        <v>-46.34</v>
+        <v>-47.04</v>
       </c>
       <c r="E13" t="n">
-        <v>-45.09</v>
+        <v>-45.44</v>
       </c>
       <c r="F13" t="n">
-        <v>-49.21</v>
+        <v>-49.34</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -5530,16 +5542,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-43.51</v>
+        <v>-45.37</v>
       </c>
       <c r="D14" t="n">
-        <v>-45.23</v>
+        <v>-46.64</v>
       </c>
       <c r="E14" t="n">
-        <v>-46.99</v>
+        <v>-47.91</v>
       </c>
       <c r="F14" t="n">
-        <v>-48.04</v>
+        <v>-48.92</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -5558,16 +5570,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-45.11</v>
+        <v>-45.33</v>
       </c>
       <c r="D15" t="n">
-        <v>-48.68</v>
+        <v>-49.16</v>
       </c>
       <c r="E15" t="n">
-        <v>-49.25</v>
+        <v>-49.71</v>
       </c>
       <c r="F15" t="n">
-        <v>-50.44</v>
+        <v>-50.83</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -5586,16 +5598,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-39.88</v>
+        <v>-39.71</v>
       </c>
       <c r="D16" t="n">
-        <v>-43.75</v>
+        <v>-43.16</v>
       </c>
       <c r="E16" t="n">
-        <v>-45.23</v>
+        <v>-44.81</v>
       </c>
       <c r="F16" t="n">
-        <v>-48.7</v>
+        <v>-48.36</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -5676,16 +5688,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-46.26</v>
+        <v>-47.32</v>
       </c>
       <c r="D2" t="n">
-        <v>-46.97</v>
+        <v>-49.13</v>
       </c>
       <c r="E2" t="n">
-        <v>-47.85</v>
+        <v>-48.24</v>
       </c>
       <c r="F2" t="n">
-        <v>-47.61</v>
+        <v>-48.47</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -5704,16 +5716,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-43.79</v>
+        <v>-47.24</v>
       </c>
       <c r="D3" t="n">
-        <v>-44.11</v>
+        <v>-47.74</v>
       </c>
       <c r="E3" t="n">
-        <v>-45.88</v>
+        <v>-48.06</v>
       </c>
       <c r="F3" t="n">
-        <v>-46.06</v>
+        <v>-48.53</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -5732,16 +5744,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-40.54</v>
+        <v>-40.06</v>
       </c>
       <c r="D4" t="n">
-        <v>-40.92</v>
+        <v>-40.96</v>
       </c>
       <c r="E4" t="n">
-        <v>-44.84</v>
+        <v>-44.02</v>
       </c>
       <c r="F4" t="n">
-        <v>-44.96</v>
+        <v>-44.73</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -5760,16 +5772,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-43.92</v>
+        <v>-45.25</v>
       </c>
       <c r="D5" t="n">
-        <v>-43.94</v>
+        <v>-45.68</v>
       </c>
       <c r="E5" t="n">
-        <v>-45.83</v>
+        <v>-46.77</v>
       </c>
       <c r="F5" t="n">
-        <v>-45.45</v>
+        <v>-46.69</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -5788,16 +5800,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-44.07</v>
+        <v>-44.35</v>
       </c>
       <c r="D6" t="n">
-        <v>-43.71</v>
+        <v>-44.06</v>
       </c>
       <c r="E6" t="n">
-        <v>-46.82</v>
+        <v>-46.74</v>
       </c>
       <c r="F6" t="n">
-        <v>-46.53</v>
+        <v>-46.49</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -5816,16 +5828,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-41.6</v>
+        <v>-44.04</v>
       </c>
       <c r="D7" t="n">
-        <v>-42.05</v>
+        <v>-45.53</v>
       </c>
       <c r="E7" t="n">
-        <v>-44.52</v>
+        <v>-45.54</v>
       </c>
       <c r="F7" t="n">
-        <v>-44.76</v>
+        <v>-46.59</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -5844,16 +5856,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-44.43</v>
+        <v>-45.31</v>
       </c>
       <c r="D8" t="n">
-        <v>-44.22</v>
+        <v>-45.15</v>
       </c>
       <c r="E8" t="n">
-        <v>-46.26</v>
+        <v>-46.94</v>
       </c>
       <c r="F8" t="n">
-        <v>-45.67</v>
+        <v>-46.4</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -5872,16 +5884,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-43.9</v>
+        <v>-44.29</v>
       </c>
       <c r="D9" t="n">
-        <v>-43.75</v>
+        <v>-44.27</v>
       </c>
       <c r="E9" t="n">
-        <v>-47.42</v>
+        <v>-47.37</v>
       </c>
       <c r="F9" t="n">
-        <v>-47.05</v>
+        <v>-47.17</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -5900,16 +5912,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-42.25</v>
+        <v>-42.6</v>
       </c>
       <c r="D10" t="n">
-        <v>-42.65</v>
+        <v>-43.66</v>
       </c>
       <c r="E10" t="n">
-        <v>-45.33</v>
+        <v>-46.17</v>
       </c>
       <c r="F10" t="n">
-        <v>-45.13</v>
+        <v>-46.49</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -5928,16 +5940,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-46.34</v>
+        <v>-44.11</v>
       </c>
       <c r="D11" t="n">
-        <v>-46.01</v>
+        <v>-43.94</v>
       </c>
       <c r="E11" t="n">
-        <v>-48.16</v>
+        <v>-46.81</v>
       </c>
       <c r="F11" t="n">
-        <v>-47.8</v>
+        <v>-46.48</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -5956,16 +5968,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-41.7</v>
+        <v>-43.51</v>
       </c>
       <c r="D12" t="n">
-        <v>-41.7</v>
+        <v>-43.43</v>
       </c>
       <c r="E12" t="n">
-        <v>-44.78</v>
+        <v>-46.34</v>
       </c>
       <c r="F12" t="n">
-        <v>-44.63</v>
+        <v>-46.24</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -5984,16 +5996,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-39.49</v>
+        <v>-40.71</v>
       </c>
       <c r="D13" t="n">
-        <v>-42.49</v>
+        <v>-43.24</v>
       </c>
       <c r="E13" t="n">
-        <v>-42.94</v>
+        <v>-44.11</v>
       </c>
       <c r="F13" t="n">
-        <v>-45.09</v>
+        <v>-46.23</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -6012,16 +6024,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-45.39</v>
+        <v>-47.23</v>
       </c>
       <c r="D14" t="n">
-        <v>-45.44</v>
+        <v>-46.68</v>
       </c>
       <c r="E14" t="n">
-        <v>-47.18</v>
+        <v>-48.83</v>
       </c>
       <c r="F14" t="n">
-        <v>-46.84</v>
+        <v>-48.24</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -6040,16 +6052,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-43.8</v>
+        <v>-44.18</v>
       </c>
       <c r="D15" t="n">
-        <v>-44.28</v>
+        <v>-44.92</v>
       </c>
       <c r="E15" t="n">
-        <v>-47.19</v>
+        <v>-47.05</v>
       </c>
       <c r="F15" t="n">
-        <v>-47.39</v>
+        <v>-47.31</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -6068,16 +6080,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-39.78</v>
+        <v>-40.03</v>
       </c>
       <c r="D16" t="n">
-        <v>-41.34</v>
+        <v>-40.95</v>
       </c>
       <c r="E16" t="n">
-        <v>-43.75</v>
+        <v>-44.06</v>
       </c>
       <c r="F16" t="n">
-        <v>-44.82</v>
+        <v>-44.87</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -6158,16 +6170,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-44.21</v>
+        <v>-47.71</v>
       </c>
       <c r="D2" t="n">
-        <v>-46.39</v>
+        <v>-49.29</v>
       </c>
       <c r="E2" t="n">
-        <v>-47.32</v>
+        <v>-49.08</v>
       </c>
       <c r="F2" t="n">
-        <v>-48.34</v>
+        <v>-49.39</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -6186,16 +6198,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-46.16</v>
+        <v>-46.77</v>
       </c>
       <c r="D3" t="n">
-        <v>-47.91</v>
+        <v>-48.48</v>
       </c>
       <c r="E3" t="n">
-        <v>-48.24</v>
+        <v>-48.58</v>
       </c>
       <c r="F3" t="n">
-        <v>-49.07</v>
+        <v>-49.2</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -6214,16 +6226,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-40.81</v>
+        <v>-39.89</v>
       </c>
       <c r="D4" t="n">
-        <v>-43.69</v>
+        <v>-43.19</v>
       </c>
       <c r="E4" t="n">
-        <v>-45.14</v>
+        <v>-44.73</v>
       </c>
       <c r="F4" t="n">
-        <v>-47.47</v>
+        <v>-47.13</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -6242,16 +6254,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-43.71</v>
+        <v>-46.93</v>
       </c>
       <c r="D5" t="n">
-        <v>-46.07</v>
+        <v>-47.71</v>
       </c>
       <c r="E5" t="n">
-        <v>-46.92</v>
+        <v>-48.14</v>
       </c>
       <c r="F5" t="n">
-        <v>-48.03</v>
+        <v>-48.19</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -6270,16 +6282,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-45.69</v>
+        <v>-42.44</v>
       </c>
       <c r="D6" t="n">
-        <v>-48.17</v>
+        <v>-44.74</v>
       </c>
       <c r="E6" t="n">
-        <v>-48.38</v>
+        <v>-46.33</v>
       </c>
       <c r="F6" t="n">
-        <v>-49.37</v>
+        <v>-47.82</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -6298,16 +6310,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-44.99</v>
+        <v>-43.78</v>
       </c>
       <c r="D7" t="n">
-        <v>-47.33</v>
+        <v>-45.74</v>
       </c>
       <c r="E7" t="n">
-        <v>-47.42</v>
+        <v>-46.81</v>
       </c>
       <c r="F7" t="n">
-        <v>-49.1</v>
+        <v>-48.2</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -6326,16 +6338,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-44.09</v>
+        <v>-43.63</v>
       </c>
       <c r="D8" t="n">
-        <v>-45.42</v>
+        <v>-45.01</v>
       </c>
       <c r="E8" t="n">
-        <v>-46.64</v>
+        <v>-46.55</v>
       </c>
       <c r="F8" t="n">
-        <v>-47.61</v>
+        <v>-47.37</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -6354,16 +6366,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-43.33</v>
+        <v>-43.61</v>
       </c>
       <c r="D9" t="n">
-        <v>-45.83</v>
+        <v>-46.43</v>
       </c>
       <c r="E9" t="n">
-        <v>-47.28</v>
+        <v>-47.57</v>
       </c>
       <c r="F9" t="n">
-        <v>-48.61</v>
+        <v>-49.18</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -6382,16 +6394,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-44.63</v>
+        <v>-42.27</v>
       </c>
       <c r="D10" t="n">
-        <v>-47.86</v>
+        <v>-44.78</v>
       </c>
       <c r="E10" t="n">
-        <v>-48.52</v>
+        <v>-46.66</v>
       </c>
       <c r="F10" t="n">
-        <v>-49.96</v>
+        <v>-48.29</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -6410,16 +6422,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-41.64</v>
+        <v>-43.27</v>
       </c>
       <c r="D11" t="n">
-        <v>-45.18</v>
+        <v>-45.09</v>
       </c>
       <c r="E11" t="n">
-        <v>-47.05</v>
+        <v>-47.39</v>
       </c>
       <c r="F11" t="n">
-        <v>-48.74</v>
+        <v>-48.45</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -6438,16 +6450,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-43.36</v>
+        <v>-42.57</v>
       </c>
       <c r="D12" t="n">
-        <v>-46.05</v>
+        <v>-44.52</v>
       </c>
       <c r="E12" t="n">
-        <v>-47.04</v>
+        <v>-46.19</v>
       </c>
       <c r="F12" t="n">
-        <v>-48.56</v>
+        <v>-47.95</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -6466,16 +6478,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-39.16</v>
+        <v>-37.91</v>
       </c>
       <c r="D13" t="n">
-        <v>-42.25</v>
+        <v>-41.09</v>
       </c>
       <c r="E13" t="n">
-        <v>-42.62</v>
+        <v>-41.3</v>
       </c>
       <c r="F13" t="n">
-        <v>-45.46</v>
+        <v>-44.78</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -6494,16 +6506,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-45.08</v>
+        <v>-44.38</v>
       </c>
       <c r="D14" t="n">
-        <v>-45.93</v>
+        <v>-45.63</v>
       </c>
       <c r="E14" t="n">
-        <v>-47.34</v>
+        <v>-47.01</v>
       </c>
       <c r="F14" t="n">
-        <v>-48.12</v>
+        <v>-47.86</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -6522,16 +6534,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-44.25</v>
+        <v>-43.61</v>
       </c>
       <c r="D15" t="n">
-        <v>-46.5</v>
+        <v>-46.35</v>
       </c>
       <c r="E15" t="n">
-        <v>-48.18</v>
+        <v>-47.94</v>
       </c>
       <c r="F15" t="n">
-        <v>-49.42</v>
+        <v>-49.47</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -6550,16 +6562,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-41.27</v>
+        <v>-39.93</v>
       </c>
       <c r="D16" t="n">
-        <v>-44.73</v>
+        <v>-42.78</v>
       </c>
       <c r="E16" t="n">
-        <v>-46.27</v>
+        <v>-44.12</v>
       </c>
       <c r="F16" t="n">
-        <v>-48.37</v>
+        <v>-46.52</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -6640,16 +6652,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-46.87</v>
+        <v>-46.1</v>
       </c>
       <c r="D2" t="n">
-        <v>-47.73</v>
+        <v>-46.91</v>
       </c>
       <c r="E2" t="n">
-        <v>-48.32</v>
+        <v>-47.86</v>
       </c>
       <c r="F2" t="n">
-        <v>-47.98</v>
+        <v>-47.57</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -6668,16 +6680,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-46.81</v>
+        <v>-44.42</v>
       </c>
       <c r="D3" t="n">
-        <v>-47</v>
+        <v>-45.33</v>
       </c>
       <c r="E3" t="n">
-        <v>-48.13</v>
+        <v>-46.42</v>
       </c>
       <c r="F3" t="n">
-        <v>-48.06</v>
+        <v>-46.99</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -6696,16 +6708,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-40.03</v>
+        <v>-40.1</v>
       </c>
       <c r="D4" t="n">
-        <v>-40.36</v>
+        <v>-40.43</v>
       </c>
       <c r="E4" t="n">
-        <v>-44.1</v>
+        <v>-43.85</v>
       </c>
       <c r="F4" t="n">
-        <v>-44.28</v>
+        <v>-44.19</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -6724,16 +6736,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-44.85</v>
+        <v>-45.17</v>
       </c>
       <c r="D5" t="n">
-        <v>-44.47</v>
+        <v>-45.51</v>
       </c>
       <c r="E5" t="n">
-        <v>-46.69</v>
+        <v>-46.59</v>
       </c>
       <c r="F5" t="n">
-        <v>-45.94</v>
+        <v>-46.39</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -6752,16 +6764,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-42.97</v>
+        <v>-45.21</v>
       </c>
       <c r="D6" t="n">
-        <v>-42.7</v>
+        <v>-44.89</v>
       </c>
       <c r="E6" t="n">
-        <v>-45.54</v>
+        <v>-47.16</v>
       </c>
       <c r="F6" t="n">
-        <v>-45.35</v>
+        <v>-46.74</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -6780,16 +6792,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-39.96</v>
+        <v>-41.93</v>
       </c>
       <c r="D7" t="n">
-        <v>-39.97</v>
+        <v>-42.88</v>
       </c>
       <c r="E7" t="n">
-        <v>-43.94</v>
+        <v>-45.31</v>
       </c>
       <c r="F7" t="n">
-        <v>-44.04</v>
+        <v>-46</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -6808,16 +6820,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-45.39</v>
+        <v>-44.22</v>
       </c>
       <c r="D8" t="n">
-        <v>-45.14</v>
+        <v>-44</v>
       </c>
       <c r="E8" t="n">
-        <v>-47.69</v>
+        <v>-46.49</v>
       </c>
       <c r="F8" t="n">
-        <v>-47.01</v>
+        <v>-45.99</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -6836,16 +6848,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-43.24</v>
+        <v>-44.99</v>
       </c>
       <c r="D9" t="n">
-        <v>-43.58</v>
+        <v>-45.07</v>
       </c>
       <c r="E9" t="n">
-        <v>-46.21</v>
+        <v>-47.2</v>
       </c>
       <c r="F9" t="n">
-        <v>-46.33</v>
+        <v>-47.14</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -6864,16 +6876,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-41.41</v>
+        <v>-41.64</v>
       </c>
       <c r="D10" t="n">
-        <v>-42.65</v>
+        <v>-42.63</v>
       </c>
       <c r="E10" t="n">
-        <v>-45.27</v>
+        <v>-45.97</v>
       </c>
       <c r="F10" t="n">
-        <v>-45.78</v>
+        <v>-46.47</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -6892,16 +6904,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-45.22</v>
+        <v>-45.9</v>
       </c>
       <c r="D11" t="n">
-        <v>-44.96</v>
+        <v>-45.73</v>
       </c>
       <c r="E11" t="n">
-        <v>-47.97</v>
+        <v>-47.95</v>
       </c>
       <c r="F11" t="n">
-        <v>-47.42</v>
+        <v>-47.37</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -6920,16 +6932,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-43.59</v>
+        <v>-42.03</v>
       </c>
       <c r="D12" t="n">
-        <v>-43.82</v>
+        <v>-41.31</v>
       </c>
       <c r="E12" t="n">
-        <v>-46.21</v>
+        <v>-45.34</v>
       </c>
       <c r="F12" t="n">
-        <v>-46.52</v>
+        <v>-44.99</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -6948,16 +6960,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-38.88</v>
+        <v>-40.11</v>
       </c>
       <c r="D13" t="n">
-        <v>-40.68</v>
+        <v>-42.46</v>
       </c>
       <c r="E13" t="n">
-        <v>-41.3</v>
+        <v>-42.84</v>
       </c>
       <c r="F13" t="n">
-        <v>-42.84</v>
+        <v>-44.8</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -6976,16 +6988,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-44.65</v>
+        <v>-44.52</v>
       </c>
       <c r="D14" t="n">
-        <v>-44.49</v>
+        <v>-44.66</v>
       </c>
       <c r="E14" t="n">
-        <v>-46.95</v>
+        <v>-46.72</v>
       </c>
       <c r="F14" t="n">
-        <v>-46.43</v>
+        <v>-46.26</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -7004,16 +7016,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-44.37</v>
+        <v>-43</v>
       </c>
       <c r="D15" t="n">
-        <v>-44.88</v>
+        <v>-43.14</v>
       </c>
       <c r="E15" t="n">
-        <v>-47.82</v>
+        <v>-46.61</v>
       </c>
       <c r="F15" t="n">
-        <v>-47.8</v>
+        <v>-46.48</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -7032,16 +7044,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-39.38</v>
+        <v>-40.04</v>
       </c>
       <c r="D16" t="n">
-        <v>-40.3</v>
+        <v>-40.82</v>
       </c>
       <c r="E16" t="n">
-        <v>-42.97</v>
+        <v>-43.59</v>
       </c>
       <c r="F16" t="n">
-        <v>-43.8</v>
+        <v>-44.26</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -7097,13 +7109,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1.25</v>
+        <v>1.14</v>
       </c>
       <c r="C2" t="n">
-        <v>1.43</v>
+        <v>1.2</v>
       </c>
       <c r="D2" t="n">
-        <v>1.38</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="3">
@@ -7111,13 +7123,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.81</v>
+        <v>1.04</v>
       </c>
       <c r="C3" t="n">
-        <v>1.23</v>
+        <v>1.12</v>
       </c>
       <c r="D3" t="n">
-        <v>1.02</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="4">
@@ -7125,13 +7137,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.03</v>
+        <v>1.16</v>
       </c>
       <c r="C4" t="n">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="D4" t="n">
-        <v>1.41</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="5">
@@ -7139,13 +7151,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>1.18</v>
+        <v>1.02</v>
       </c>
       <c r="C5" t="n">
-        <v>1.02</v>
+        <v>1.27</v>
       </c>
       <c r="D5" t="n">
-        <v>1.63</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="6">
@@ -7153,13 +7165,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>1.21</v>
+        <v>1.25</v>
       </c>
       <c r="C6" t="n">
-        <v>1.17</v>
+        <v>1.35</v>
       </c>
       <c r="D6" t="n">
-        <v>1.9</v>
+        <v>1.77</v>
       </c>
     </row>
   </sheetData>
@@ -7209,13 +7221,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1.38</v>
+        <v>1.16</v>
       </c>
       <c r="C2" t="n">
-        <v>1.52</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.74</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="3">
@@ -7223,13 +7235,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.15</v>
+        <v>1.26</v>
       </c>
       <c r="C3" t="n">
-        <v>1.39</v>
+        <v>1.31</v>
       </c>
       <c r="D3" t="n">
-        <v>1.39</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="4">
@@ -7237,13 +7249,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.26</v>
+        <v>0.99</v>
       </c>
       <c r="C4" t="n">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="D4" t="n">
-        <v>1.37</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="5">
@@ -7251,13 +7263,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>1.35</v>
+        <v>1.13</v>
       </c>
       <c r="C5" t="n">
-        <v>1.53</v>
+        <v>1.15</v>
       </c>
       <c r="D5" t="n">
-        <v>1.36</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="6">
@@ -7265,13 +7277,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>1.05</v>
+        <v>1.15</v>
       </c>
       <c r="C6" t="n">
         <v>1.3</v>
       </c>
       <c r="D6" t="n">
-        <v>2.09</v>
+        <v>1.93</v>
       </c>
     </row>
   </sheetData>
@@ -7321,13 +7333,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1.31</v>
+        <v>1.27</v>
       </c>
       <c r="C2" t="n">
-        <v>1.39</v>
+        <v>1.71</v>
       </c>
       <c r="D2" t="n">
-        <v>2.06</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="3">
@@ -7335,13 +7347,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.68</v>
+        <v>1.76</v>
       </c>
       <c r="C3" t="n">
-        <v>1.48</v>
+        <v>2.21</v>
       </c>
       <c r="D3" t="n">
-        <v>1.3</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="4">
@@ -7349,13 +7361,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.25</v>
+        <v>1.72</v>
       </c>
       <c r="C4" t="n">
-        <v>1.64</v>
+        <v>1.56</v>
       </c>
       <c r="D4" t="n">
-        <v>1.98</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="5">
@@ -7363,13 +7375,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>1.36</v>
+        <v>1.76</v>
       </c>
       <c r="C5" t="n">
-        <v>1.22</v>
+        <v>1.25</v>
       </c>
       <c r="D5" t="n">
-        <v>1.78</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="6">
@@ -7377,13 +7389,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>1.27</v>
+        <v>1.4</v>
       </c>
       <c r="C6" t="n">
-        <v>1.47</v>
+        <v>1.49</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>2.22</v>
       </c>
     </row>
   </sheetData>
@@ -7433,13 +7445,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1.37</v>
+        <v>1.21</v>
       </c>
       <c r="C2" t="n">
-        <v>2.26</v>
+        <v>1.59</v>
       </c>
       <c r="D2" t="n">
-        <v>2.06</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="3">
@@ -7447,13 +7459,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.43</v>
+        <v>1.73</v>
       </c>
       <c r="C3" t="n">
-        <v>1.65</v>
+        <v>1.51</v>
       </c>
       <c r="D3" t="n">
-        <v>1.27</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="4">
@@ -7461,13 +7473,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.69</v>
+        <v>1.22</v>
       </c>
       <c r="C4" t="n">
-        <v>1.8</v>
+        <v>1.63</v>
       </c>
       <c r="D4" t="n">
-        <v>1.53</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="5">
@@ -7475,13 +7487,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>1.78</v>
+        <v>1.46</v>
       </c>
       <c r="C5" t="n">
-        <v>1.6</v>
+        <v>1.57</v>
       </c>
       <c r="D5" t="n">
-        <v>1.86</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="6">
@@ -7489,13 +7501,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>1.41</v>
+        <v>1.43</v>
       </c>
       <c r="C6" t="n">
-        <v>1.53</v>
+        <v>1.44</v>
       </c>
       <c r="D6" t="n">
-        <v>1.79</v>
+        <v>2.01</v>
       </c>
     </row>
   </sheetData>
@@ -7545,13 +7557,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1.58</v>
+        <v>1.22</v>
       </c>
       <c r="C2" t="n">
-        <v>2.46</v>
+        <v>1.27</v>
       </c>
       <c r="D2" t="n">
-        <v>5.28</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="3">
@@ -7559,13 +7571,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>2.29</v>
+        <v>1.28</v>
       </c>
       <c r="C3" t="n">
-        <v>1.64</v>
+        <v>2.21</v>
       </c>
       <c r="D3" t="n">
-        <v>9.039999999999999</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="4">
@@ -7573,13 +7585,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>3.6</v>
+        <v>1.35</v>
       </c>
       <c r="C4" t="n">
-        <v>11.49</v>
+        <v>1.83</v>
       </c>
       <c r="D4" t="n">
-        <v>10.9</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="5">
@@ -7587,13 +7599,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>2.63</v>
+        <v>1.8</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>1.91</v>
       </c>
       <c r="D5" t="n">
-        <v>11.12</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="6">
@@ -7601,13 +7613,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>3.11</v>
+        <v>1.46</v>
       </c>
       <c r="C6" t="n">
-        <v>1.81</v>
+        <v>2.14</v>
       </c>
       <c r="D6" t="n">
-        <v>2.04</v>
+        <v>2.22</v>
       </c>
     </row>
   </sheetData>
@@ -7657,13 +7669,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1.46</v>
+        <v>1.54</v>
       </c>
       <c r="C2" t="n">
-        <v>9.26</v>
+        <v>1.54</v>
       </c>
       <c r="D2" t="n">
-        <v>2.18</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="3">
@@ -7671,13 +7683,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.58</v>
+        <v>1.32</v>
       </c>
       <c r="C3" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="D3" t="n">
         <v>1.81</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2.05</v>
       </c>
     </row>
     <row r="4">
@@ -7685,13 +7697,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.91</v>
+        <v>1.51</v>
       </c>
       <c r="C4" t="n">
-        <v>3.42</v>
+        <v>1.67</v>
       </c>
       <c r="D4" t="n">
-        <v>1.95</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="5">
@@ -7699,13 +7711,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>11.05</v>
+        <v>1.47</v>
       </c>
       <c r="C5" t="n">
-        <v>2.17</v>
+        <v>2.18</v>
       </c>
       <c r="D5" t="n">
-        <v>2.18</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="6">
@@ -7713,13 +7725,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>1.55</v>
+        <v>1.38</v>
       </c>
       <c r="C6" t="n">
-        <v>1.62</v>
+        <v>1.47</v>
       </c>
       <c r="D6" t="n">
-        <v>2.02</v>
+        <v>2.09</v>
       </c>
     </row>
   </sheetData>
@@ -7769,13 +7781,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>24.59</v>
+        <v>24.41</v>
       </c>
       <c r="C2" t="n">
-        <v>24.71</v>
+        <v>24.23</v>
       </c>
       <c r="D2" t="n">
-        <v>24.61</v>
+        <v>24.15</v>
       </c>
     </row>
     <row r="3">
@@ -7783,13 +7795,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>24.81</v>
+        <v>24.27</v>
       </c>
       <c r="C3" t="n">
-        <v>24.8</v>
+        <v>24.36</v>
       </c>
       <c r="D3" t="n">
-        <v>24.76</v>
+        <v>24.48</v>
       </c>
     </row>
     <row r="4">
@@ -7797,13 +7809,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>24.55</v>
+        <v>24</v>
       </c>
       <c r="C4" t="n">
-        <v>24.45</v>
+        <v>23.88</v>
       </c>
       <c r="D4" t="n">
-        <v>24.55</v>
+        <v>23.88</v>
       </c>
     </row>
     <row r="5">
@@ -7811,13 +7823,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>24.66</v>
+        <v>24.35</v>
       </c>
       <c r="C5" t="n">
-        <v>24.68</v>
+        <v>24.3</v>
       </c>
       <c r="D5" t="n">
-        <v>24.57</v>
+        <v>24.12</v>
       </c>
     </row>
     <row r="6">
@@ -7825,13 +7837,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>24.88</v>
+        <v>24.21</v>
       </c>
       <c r="C6" t="n">
-        <v>24.85</v>
+        <v>24.33</v>
       </c>
       <c r="D6" t="n">
-        <v>24.87</v>
+        <v>24.28</v>
       </c>
     </row>
   </sheetData>
@@ -7881,13 +7893,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>23.76</v>
+        <v>23.36</v>
       </c>
       <c r="C2" t="n">
-        <v>23.69</v>
+        <v>23.27</v>
       </c>
       <c r="D2" t="n">
-        <v>23.76</v>
+        <v>23.31</v>
       </c>
     </row>
     <row r="3">
@@ -7895,13 +7907,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>23.86</v>
+        <v>23.23</v>
       </c>
       <c r="C3" t="n">
-        <v>23.85</v>
+        <v>23.47</v>
       </c>
       <c r="D3" t="n">
-        <v>23.77</v>
+        <v>23.46</v>
       </c>
     </row>
     <row r="4">
@@ -7909,13 +7921,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>23.52</v>
+        <v>22.99</v>
       </c>
       <c r="C4" t="n">
-        <v>23.51</v>
+        <v>22.86</v>
       </c>
       <c r="D4" t="n">
-        <v>23.6</v>
+        <v>22.87</v>
       </c>
     </row>
     <row r="5">
@@ -7923,13 +7935,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>23.69</v>
+        <v>23.31</v>
       </c>
       <c r="C5" t="n">
-        <v>23.78</v>
+        <v>23.34</v>
       </c>
       <c r="D5" t="n">
-        <v>23.56</v>
+        <v>23.22</v>
       </c>
     </row>
     <row r="6">
@@ -7937,13 +7949,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>23.82</v>
+        <v>23.15</v>
       </c>
       <c r="C6" t="n">
-        <v>23.83</v>
+        <v>23.21</v>
       </c>
       <c r="D6" t="n">
-        <v>23.85</v>
+        <v>23.16</v>
       </c>
     </row>
   </sheetData>
@@ -7993,13 +8005,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>23.75</v>
+        <v>23.33</v>
       </c>
       <c r="C2" t="n">
-        <v>23.95</v>
+        <v>23.48</v>
       </c>
       <c r="D2" t="n">
-        <v>23.35</v>
+        <v>23.28</v>
       </c>
     </row>
     <row r="3">
@@ -8007,13 +8019,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>23.95</v>
+        <v>23.39</v>
       </c>
       <c r="C3" t="n">
-        <v>23.92</v>
+        <v>23.48</v>
       </c>
       <c r="D3" t="n">
-        <v>23.82</v>
+        <v>23.49</v>
       </c>
     </row>
     <row r="4">
@@ -8021,13 +8033,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>23.62</v>
+        <v>23.03</v>
       </c>
       <c r="C4" t="n">
-        <v>23.23</v>
+        <v>22.82</v>
       </c>
       <c r="D4" t="n">
-        <v>23.65</v>
+        <v>23.2</v>
       </c>
     </row>
     <row r="5">
@@ -8035,13 +8047,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>23.76</v>
+        <v>23.42</v>
       </c>
       <c r="C5" t="n">
-        <v>23.64</v>
+        <v>23.48</v>
       </c>
       <c r="D5" t="n">
-        <v>23.52</v>
+        <v>23.21</v>
       </c>
     </row>
     <row r="6">
@@ -8049,13 +8061,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>23.78</v>
+        <v>23.31</v>
       </c>
       <c r="C6" t="n">
-        <v>23.58</v>
+        <v>23.18</v>
       </c>
       <c r="D6" t="n">
-        <v>23.87</v>
+        <v>23.33</v>
       </c>
     </row>
   </sheetData>
@@ -8105,13 +8117,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>21.9</v>
+        <v>21.24</v>
       </c>
       <c r="C2" t="n">
-        <v>21.91</v>
+        <v>21.39</v>
       </c>
       <c r="D2" t="n">
-        <v>21.84</v>
+        <v>21.38</v>
       </c>
     </row>
     <row r="3">
@@ -8119,13 +8131,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>22.86</v>
+        <v>22.37</v>
       </c>
       <c r="C3" t="n">
-        <v>23.07</v>
+        <v>22.39</v>
       </c>
       <c r="D3" t="n">
-        <v>22.83</v>
+        <v>22.43</v>
       </c>
     </row>
     <row r="4">
@@ -8133,13 +8145,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>22.47</v>
+        <v>21.91</v>
       </c>
       <c r="C4" t="n">
-        <v>22.54</v>
+        <v>21.78</v>
       </c>
       <c r="D4" t="n">
-        <v>22.61</v>
+        <v>21.91</v>
       </c>
     </row>
     <row r="5">
@@ -8147,13 +8159,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>22.65</v>
+        <v>22.2</v>
       </c>
       <c r="C5" t="n">
-        <v>22.71</v>
+        <v>22.19</v>
       </c>
       <c r="D5" t="n">
-        <v>22.66</v>
+        <v>22.16</v>
       </c>
     </row>
     <row r="6">
@@ -8161,13 +8173,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>21.76</v>
+        <v>21.23</v>
       </c>
       <c r="C6" t="n">
-        <v>21.95</v>
+        <v>21.31</v>
       </c>
       <c r="D6" t="n">
-        <v>21.79</v>
+        <v>21.12</v>
       </c>
     </row>
   </sheetData>
@@ -8217,13 +8229,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>22.62</v>
+        <v>22.25</v>
       </c>
       <c r="C2" t="n">
-        <v>22.63</v>
+        <v>22.25</v>
       </c>
       <c r="D2" t="n">
-        <v>22.69</v>
+        <v>22.33</v>
       </c>
     </row>
     <row r="3">
@@ -8231,13 +8243,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>22.97</v>
+        <v>22.43</v>
       </c>
       <c r="C3" t="n">
-        <v>22.93</v>
+        <v>22.46</v>
       </c>
       <c r="D3" t="n">
-        <v>22.74</v>
+        <v>22.63</v>
       </c>
     </row>
     <row r="4">
@@ -8245,13 +8257,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>22.45</v>
+        <v>22.09</v>
       </c>
       <c r="C4" t="n">
-        <v>22.51</v>
+        <v>22.01</v>
       </c>
       <c r="D4" t="n">
-        <v>22.61</v>
+        <v>22.04</v>
       </c>
     </row>
     <row r="5">
@@ -8259,13 +8271,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>22.74</v>
+        <v>22.51</v>
       </c>
       <c r="C5" t="n">
-        <v>22.52</v>
+        <v>22.46</v>
       </c>
       <c r="D5" t="n">
-        <v>22.76</v>
+        <v>22.48</v>
       </c>
     </row>
     <row r="6">
@@ -8273,13 +8285,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>22.91</v>
+        <v>22.18</v>
       </c>
       <c r="C6" t="n">
-        <v>22.78</v>
+        <v>22.64</v>
       </c>
       <c r="D6" t="n">
-        <v>22.69</v>
+        <v>22.41</v>
       </c>
     </row>
   </sheetData>
@@ -8329,13 +8341,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>21.8</v>
+        <v>21.27</v>
       </c>
       <c r="C2" t="n">
-        <v>21.77</v>
+        <v>21.19</v>
       </c>
       <c r="D2" t="n">
-        <v>21.7</v>
+        <v>21.28</v>
       </c>
     </row>
     <row r="3">
@@ -8343,13 +8355,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>21.93</v>
+        <v>21.4</v>
       </c>
       <c r="C3" t="n">
-        <v>22.04</v>
+        <v>21.72</v>
       </c>
       <c r="D3" t="n">
-        <v>21.99</v>
+        <v>21.41</v>
       </c>
     </row>
     <row r="4">
@@ -8357,13 +8369,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>21.77</v>
+        <v>20.91</v>
       </c>
       <c r="C4" t="n">
-        <v>21.61</v>
+        <v>20.69</v>
       </c>
       <c r="D4" t="n">
-        <v>21.67</v>
+        <v>20.97</v>
       </c>
     </row>
     <row r="5">
@@ -8371,13 +8383,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>21.72</v>
+        <v>21.45</v>
       </c>
       <c r="C5" t="n">
-        <v>21.75</v>
+        <v>21.39</v>
       </c>
       <c r="D5" t="n">
-        <v>21.93</v>
+        <v>21.35</v>
       </c>
     </row>
     <row r="6">
@@ -8385,13 +8397,13 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>21.88</v>
+        <v>21.19</v>
       </c>
       <c r="C6" t="n">
-        <v>21.98</v>
+        <v>21.24</v>
       </c>
       <c r="D6" t="n">
-        <v>21.83</v>
+        <v>20.92</v>
       </c>
     </row>
   </sheetData>
@@ -8466,16 +8478,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-47.47</v>
+        <v>-47.06</v>
       </c>
       <c r="D2" t="n">
-        <v>-49.7</v>
+        <v>-48.91</v>
       </c>
       <c r="E2" t="n">
-        <v>-49.5</v>
+        <v>-49.23</v>
       </c>
       <c r="F2" t="n">
-        <v>-50.56</v>
+        <v>-50.16</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -8494,16 +8506,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-48.55</v>
+        <v>-46.96</v>
       </c>
       <c r="D3" t="n">
-        <v>-50.24</v>
+        <v>-48.85</v>
       </c>
       <c r="E3" t="n">
-        <v>-50.02</v>
+        <v>-49.14</v>
       </c>
       <c r="F3" t="n">
-        <v>-51.07</v>
+        <v>-50.56</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -8522,16 +8534,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-42.28</v>
+        <v>-42.79</v>
       </c>
       <c r="D4" t="n">
-        <v>-44.94</v>
+        <v>-45.05</v>
       </c>
       <c r="E4" t="n">
-        <v>-46.68</v>
+        <v>-47.03</v>
       </c>
       <c r="F4" t="n">
-        <v>-48.53</v>
+        <v>-48.92</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -8550,16 +8562,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-48.53</v>
+        <v>-46.53</v>
       </c>
       <c r="D5" t="n">
-        <v>-49.84</v>
+        <v>-47.77</v>
       </c>
       <c r="E5" t="n">
-        <v>-50.19</v>
+        <v>-48.76</v>
       </c>
       <c r="F5" t="n">
-        <v>-50.27</v>
+        <v>-49.09</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -8578,16 +8590,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-46.47</v>
+        <v>-43.83</v>
       </c>
       <c r="D6" t="n">
-        <v>-48.45</v>
+        <v>-46</v>
       </c>
       <c r="E6" t="n">
-        <v>-49.39</v>
+        <v>-47.65</v>
       </c>
       <c r="F6" t="n">
-        <v>-50.6</v>
+        <v>-49.55</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -8606,16 +8618,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-45.75</v>
+        <v>-48.82</v>
       </c>
       <c r="D7" t="n">
-        <v>-47.36</v>
+        <v>-49.7</v>
       </c>
       <c r="E7" t="n">
-        <v>-47.88</v>
+        <v>-49.97</v>
       </c>
       <c r="F7" t="n">
-        <v>-49.68</v>
+        <v>-51.09</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -8634,16 +8646,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-49.41</v>
+        <v>-48.94</v>
       </c>
       <c r="D8" t="n">
-        <v>-50.36</v>
+        <v>-50.76</v>
       </c>
       <c r="E8" t="n">
-        <v>-50.56</v>
+        <v>-50.61</v>
       </c>
       <c r="F8" t="n">
-        <v>-50.96</v>
+        <v>-51.11</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -8662,16 +8674,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-44.7</v>
+        <v>-44.65</v>
       </c>
       <c r="D9" t="n">
-        <v>-47.9</v>
+        <v>-47.87</v>
       </c>
       <c r="E9" t="n">
-        <v>-48.78</v>
+        <v>-48.77</v>
       </c>
       <c r="F9" t="n">
-        <v>-50.15</v>
+        <v>-50.08</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -8690,16 +8702,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-44.27</v>
+        <v>-42.65</v>
       </c>
       <c r="D10" t="n">
-        <v>-48.2</v>
+        <v>-46.71</v>
       </c>
       <c r="E10" t="n">
-        <v>-48.58</v>
+        <v>-47.81</v>
       </c>
       <c r="F10" t="n">
-        <v>-50.71</v>
+        <v>-50.45</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -8718,16 +8730,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-48.91</v>
+        <v>-46.91</v>
       </c>
       <c r="D11" t="n">
-        <v>-50.18</v>
+        <v>-48.48</v>
       </c>
       <c r="E11" t="n">
-        <v>-50.23</v>
+        <v>-49.07</v>
       </c>
       <c r="F11" t="n">
-        <v>-50.74</v>
+        <v>-49.97</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -8746,16 +8758,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-48.54</v>
+        <v>-47.97</v>
       </c>
       <c r="D12" t="n">
-        <v>-49.86</v>
+        <v>-49.55</v>
       </c>
       <c r="E12" t="n">
-        <v>-49.84</v>
+        <v>-49.7</v>
       </c>
       <c r="F12" t="n">
-        <v>-50.88</v>
+        <v>-50.81</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -8774,16 +8786,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-41.17</v>
+        <v>-40.15</v>
       </c>
       <c r="D13" t="n">
-        <v>-45.24</v>
+        <v>-43.74</v>
       </c>
       <c r="E13" t="n">
-        <v>-43.8</v>
+        <v>-43.36</v>
       </c>
       <c r="F13" t="n">
-        <v>-48.32</v>
+        <v>-47.47</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -8802,16 +8814,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-50.38</v>
+        <v>-46.85</v>
       </c>
       <c r="D14" t="n">
-        <v>-50.73</v>
+        <v>-47.84</v>
       </c>
       <c r="E14" t="n">
-        <v>-51.07</v>
+        <v>-49.05</v>
       </c>
       <c r="F14" t="n">
-        <v>-51.04</v>
+        <v>-49.68</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -8830,16 +8842,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-45.83</v>
+        <v>-45.88</v>
       </c>
       <c r="D15" t="n">
-        <v>-48.36</v>
+        <v>-49.21</v>
       </c>
       <c r="E15" t="n">
-        <v>-49.71</v>
+        <v>-49.69</v>
       </c>
       <c r="F15" t="n">
-        <v>-51.23</v>
+        <v>-51.19</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -8858,16 +8870,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-39.23</v>
+        <v>-39.28</v>
       </c>
       <c r="D16" t="n">
-        <v>-42.65</v>
+        <v>-42.11</v>
       </c>
       <c r="E16" t="n">
-        <v>-43.7</v>
+        <v>-43.26</v>
       </c>
       <c r="F16" t="n">
-        <v>-47.31</v>
+        <v>-46.42</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -8948,16 +8960,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-45.91</v>
+        <v>-47.99</v>
       </c>
       <c r="D2" t="n">
-        <v>-46.72</v>
+        <v>-49.51</v>
       </c>
       <c r="E2" t="n">
-        <v>-47.57</v>
+        <v>-48.94</v>
       </c>
       <c r="F2" t="n">
-        <v>-47.66</v>
+        <v>-49.16</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -8976,16 +8988,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-49.06</v>
+        <v>-48.01</v>
       </c>
       <c r="D3" t="n">
-        <v>-49.26</v>
+        <v>-48.2</v>
       </c>
       <c r="E3" t="n">
-        <v>-49.72</v>
+        <v>-49.25</v>
       </c>
       <c r="F3" t="n">
-        <v>-49.76</v>
+        <v>-49.11</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -9004,16 +9016,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-41.83</v>
+        <v>-42.99</v>
       </c>
       <c r="D4" t="n">
-        <v>-41.84</v>
+        <v>-43.27</v>
       </c>
       <c r="E4" t="n">
-        <v>-45.32</v>
+        <v>-46.42</v>
       </c>
       <c r="F4" t="n">
-        <v>-45.26</v>
+        <v>-46.25</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -9032,16 +9044,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-48.27</v>
+        <v>-45.34</v>
       </c>
       <c r="D5" t="n">
-        <v>-48.4</v>
+        <v>-45.25</v>
       </c>
       <c r="E5" t="n">
-        <v>-49</v>
+        <v>-47.13</v>
       </c>
       <c r="F5" t="n">
-        <v>-48.69</v>
+        <v>-46.4</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -9060,16 +9072,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-45.85</v>
+        <v>-46.22</v>
       </c>
       <c r="D6" t="n">
-        <v>-45.54</v>
+        <v>-46.32</v>
       </c>
       <c r="E6" t="n">
+        <v>-48.32</v>
+      </c>
+      <c r="F6" t="n">
         <v>-48.13</v>
-      </c>
-      <c r="F6" t="n">
-        <v>-48.06</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -9088,16 +9100,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-45.72</v>
+        <v>-47.35</v>
       </c>
       <c r="D7" t="n">
-        <v>-46.12</v>
+        <v>-47.56</v>
       </c>
       <c r="E7" t="n">
-        <v>-46.94</v>
+        <v>-48.4</v>
       </c>
       <c r="F7" t="n">
-        <v>-47.51</v>
+        <v>-48.81</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -9116,16 +9128,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-49.27</v>
+        <v>-48.38</v>
       </c>
       <c r="D8" t="n">
-        <v>-49.12</v>
+        <v>-48.13</v>
       </c>
       <c r="E8" t="n">
-        <v>-49.94</v>
+        <v>-49.76</v>
       </c>
       <c r="F8" t="n">
-        <v>-49.2</v>
+        <v>-49.09</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -9144,16 +9156,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-45.98</v>
+        <v>-44.28</v>
       </c>
       <c r="D9" t="n">
-        <v>-46.41</v>
+        <v>-44.95</v>
       </c>
       <c r="E9" t="n">
-        <v>-48.37</v>
+        <v>-46.78</v>
       </c>
       <c r="F9" t="n">
-        <v>-48.24</v>
+        <v>-47.07</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -9172,16 +9184,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-42.43</v>
+        <v>-41.67</v>
       </c>
       <c r="D10" t="n">
-        <v>-43.51</v>
+        <v>-42.84</v>
       </c>
       <c r="E10" t="n">
-        <v>-45.57</v>
+        <v>-45.48</v>
       </c>
       <c r="F10" t="n">
-        <v>-45.88</v>
+        <v>-45.97</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -9200,16 +9212,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-46.55</v>
+        <v>-44.94</v>
       </c>
       <c r="D11" t="n">
-        <v>-46.36</v>
+        <v>-44.83</v>
       </c>
       <c r="E11" t="n">
-        <v>-48.19</v>
+        <v>-46.96</v>
       </c>
       <c r="F11" t="n">
-        <v>-47.62</v>
+        <v>-46.64</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -9228,16 +9240,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-45.74</v>
+        <v>-48.44</v>
       </c>
       <c r="D12" t="n">
-        <v>-45.85</v>
+        <v>-47.8</v>
       </c>
       <c r="E12" t="n">
-        <v>-47.46</v>
+        <v>-49.62</v>
       </c>
       <c r="F12" t="n">
-        <v>-47.59</v>
+        <v>-49.48</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -9256,16 +9268,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-43.23</v>
+        <v>-42.74</v>
       </c>
       <c r="D13" t="n">
-        <v>-47.36</v>
+        <v>-46.18</v>
       </c>
       <c r="E13" t="n">
-        <v>-45.11</v>
+        <v>-44.57</v>
       </c>
       <c r="F13" t="n">
-        <v>-48.5</v>
+        <v>-47.66</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -9284,16 +9296,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-49.28</v>
+        <v>-48.85</v>
       </c>
       <c r="D14" t="n">
-        <v>-48.97</v>
+        <v>-48.52</v>
       </c>
       <c r="E14" t="n">
-        <v>-49.84</v>
+        <v>-50.13</v>
       </c>
       <c r="F14" t="n">
-        <v>-49.09</v>
+        <v>-49.27</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -9312,16 +9324,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-44.05</v>
+        <v>-43.5</v>
       </c>
       <c r="D15" t="n">
-        <v>-44.73</v>
+        <v>-44.6</v>
       </c>
       <c r="E15" t="n">
-        <v>-47.31</v>
+        <v>-46.97</v>
       </c>
       <c r="F15" t="n">
-        <v>-47.39</v>
+        <v>-47.58</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -9340,16 +9352,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-39.88</v>
+        <v>-39.76</v>
       </c>
       <c r="D16" t="n">
-        <v>-41.4</v>
+        <v>-41.46</v>
       </c>
       <c r="E16" t="n">
-        <v>-44.24</v>
+        <v>-44.85</v>
       </c>
       <c r="F16" t="n">
-        <v>-45.62</v>
+        <v>-46.35</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>

</xml_diff>